<commit_message>
Mais suporte a unidades
</commit_message>
<xml_diff>
--- a/Unidades.xlsx
+++ b/Unidades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -747,12 +747,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -767,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -796,6 +802,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1708,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2065,7 @@
       <c r="D19" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="11">
         <v>63.614907234075197</v>
       </c>
       <c r="F19" s="3">
@@ -2709,15 +2718,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:A29"/>
     <mergeCell ref="A34:A45"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>